<commit_message>
Subscribe Crate via API
</commit_message>
<xml_diff>
--- a/Crate/TC_MobileTemplate/Main.rvl.xlsx
+++ b/Crate/TC_MobileTemplate/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Flow</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Robin</t>
+  </si>
+  <si>
+    <t>robin@crate.com</t>
+  </si>
+  <si>
+    <t>UserPassword</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -509,18 +518,26 @@
         <v>11</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="32"/>
     </row>
     <row r="5">
       <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" s="35"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="E5" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>18</v>
+      </c>
       <c r="H5" s="40"/>
     </row>
     <row r="6">

</xml_diff>